<commit_message>
updated image preprocessing script to create rotated imgs
</commit_message>
<xml_diff>
--- a/20210501 Tennis Court Detection Test Results.xlsx
+++ b/20210501 Tennis Court Detection Test Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00ae3f07a1e700d/Documents/01_Repo/opencv-play/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="378" documentId="8_{2D7FC5CA-3D0C-4B5A-B7FB-375324B2700F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7FBEA8C6-620E-4157-B153-9AD689652195}"/>
+  <xr:revisionPtr revIDLastSave="379" documentId="8_{2D7FC5CA-3D0C-4B5A-B7FB-375324B2700F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC1B8EFC-B769-462A-BA2B-547980434521}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
   <si>
     <t>Comments</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Set2 positives are all zoomed in on a single tennis court. Images were scaled/cropped and converted to BW</t>
+  </si>
+  <si>
+    <t>Set2b: manually added more pos and negs. Also processed images to duplicate each multiple times with small rotations</t>
   </si>
 </sst>
 </file>
@@ -1096,6 +1099,9 @@
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B11)</f>
         <v>0</v>
       </c>
+      <c r="P11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="15">

</xml_diff>

<commit_message>
reorganized file structure and updated README
</commit_message>
<xml_diff>
--- a/20210501 Tennis Court Detection Test Results.xlsx
+++ b/20210501 Tennis Court Detection Test Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a00ae3f07a1e700d/Documents/01_Repo/opencv-play/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="8_{2D7FC5CA-3D0C-4B5A-B7FB-375324B2700F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC1B8EFC-B769-462A-BA2B-547980434521}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="8_{2D7FC5CA-3D0C-4B5A-B7FB-375324B2700F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1C06A4E7-DC47-4EE0-84CE-702295D020CA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="50">
   <si>
     <t>Comments</t>
   </si>
@@ -171,7 +171,19 @@
     <t>Set2 positives are all zoomed in on a single tennis court. Images were scaled/cropped and converted to BW</t>
   </si>
   <si>
-    <t>Set2b: manually added more pos and negs. Also processed images to duplicate each multiple times with small rotations</t>
+    <t>Set2b</t>
+  </si>
+  <si>
+    <t>Reduce image sizes to 20x40</t>
+  </si>
+  <si>
+    <t>Set2b: manually added more pos and negs. Also processed images to duplicate each multiple times with small rotations. Positive image usage % set to 90% due to BadArgumentError (?). Image dimensions 60 x 114</t>
+  </si>
+  <si>
+    <t>MinNeighbors</t>
+  </si>
+  <si>
+    <t>Check Rotations?</t>
   </si>
 </sst>
 </file>
@@ -255,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +307,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1E8F8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -430,6 +454,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,6 +470,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF1E8F8"/>
       <color rgb="FFE4F6FC"/>
       <color rgb="FF525252"/>
       <color rgb="FF1999C1"/>
@@ -448,7 +480,6 @@
       <color rgb="FFFAC1B8"/>
       <color rgb="FFC5F3CD"/>
       <color rgb="FFE6F1DF"/>
-      <color rgb="FFFCEFD8"/>
     </mruColors>
   </colors>
   <extLst>
@@ -808,7 +839,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95065D9-21E2-4631-8E00-95D37F7A67C6}">
-  <dimension ref="B1:P15"/>
+  <dimension ref="B1:R15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
@@ -816,26 +847,27 @@
   <cols>
     <col min="1" max="1" width="2.6328125" customWidth="1"/>
     <col min="2" max="2" width="3.6328125" customWidth="1"/>
-    <col min="3" max="4" width="16.6328125" customWidth="1"/>
-    <col min="5" max="11" width="15.6328125" customWidth="1"/>
-    <col min="12" max="15" width="12.6328125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="40.6328125" customWidth="1" collapsed="1"/>
-    <col min="17" max="19" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="13" width="15.6328125" customWidth="1"/>
+    <col min="14" max="17" width="12.6328125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="40.6328125" customWidth="1" collapsed="1"/>
+    <col min="19" max="21" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:18" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="B1" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:18" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
       <c r="E4" s="20" t="s">
         <v>20</v>
       </c>
@@ -843,22 +875,24 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
       <c r="O4" s="21"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="E6" s="24" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="24"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
@@ -883,29 +917,35 @@
       <c r="I7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="M7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="N7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="O7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="P7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="Q7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="R7" s="30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="15">
         <v>1</v>
       </c>
@@ -930,35 +970,37 @@
       <c r="I8" s="27">
         <v>32</v>
       </c>
-      <c r="J8" s="23">
-        <f>IFERROR(L8/(L8+M8),"-")</f>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="23">
+        <f>IFERROR(N8/(N8+O8),"-")</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="K8" s="23">
-        <f>IFERROR(L8/(L8+O8),"-")</f>
+      <c r="M8" s="23">
+        <f>IFERROR(N8/(N8+Q8),"-")</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="L8" s="22">
+      <c r="N8" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$135,Test_Logs!$B$9:$B$135,$B8)</f>
         <v>2</v>
       </c>
-      <c r="M8" s="22">
+      <c r="O8" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$135,Test_Logs!$B$9:$B$135,$B8)</f>
         <v>5</v>
       </c>
-      <c r="N8" s="22">
+      <c r="P8" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$135,Test_Logs!$B$9:$B$135,$B8)</f>
         <v>4</v>
       </c>
-      <c r="O8" s="22">
+      <c r="Q8" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B8)</f>
         <v>7</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B9" s="15">
         <v>2</v>
       </c>
@@ -983,35 +1025,37 @@
       <c r="I9" s="27">
         <v>24</v>
       </c>
-      <c r="J9" s="23" t="str">
-        <f t="shared" ref="J9:J15" si="0">IFERROR(L9/(L9+M9),"-")</f>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="23" t="str">
+        <f t="shared" ref="L9:L15" si="0">IFERROR(N9/(N9+O9),"-")</f>
         <v>-</v>
       </c>
-      <c r="K9" s="23">
-        <f t="shared" ref="K9:K15" si="1">IFERROR(L9/(L9+O9),"-")</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="22">
+      <c r="M9" s="23">
+        <f t="shared" ref="M9:M15" si="1">IFERROR(N9/(N9+Q9),"-")</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$135,Test_Logs!$B$9:$B$135,$B9)</f>
         <v>0</v>
       </c>
-      <c r="M9" s="22">
+      <c r="O9" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$135,Test_Logs!$B$9:$B$135,$B9)</f>
         <v>0</v>
       </c>
-      <c r="N9" s="22">
+      <c r="P9" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$135,Test_Logs!$B$9:$B$135,$B9)</f>
         <v>10</v>
       </c>
-      <c r="O9" s="22">
+      <c r="Q9" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B9)</f>
         <v>18</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B10" s="15">
         <v>3</v>
       </c>
@@ -1036,74 +1080,86 @@
       <c r="I10" s="27">
         <v>48</v>
       </c>
-      <c r="J10" s="23" t="str">
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="23" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="K10" s="23" t="str">
+      <c r="M10" s="23" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L10" s="22">
+      <c r="N10" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$135,Test_Logs!$B$9:$B$135,$B10)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="22">
+      <c r="O10" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$135,Test_Logs!$B$9:$B$135,$B10)</f>
         <v>0</v>
       </c>
-      <c r="N10" s="22">
+      <c r="P10" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$135,Test_Logs!$B$9:$B$135,$B10)</f>
         <v>0</v>
       </c>
-      <c r="O10" s="22">
+      <c r="Q10" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B10)</f>
         <v>0</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B11" s="15">
         <v>4</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="32"/>
+      <c r="D11" s="32" t="s">
+        <v>45</v>
+      </c>
       <c r="E11" s="26"/>
       <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="23" t="str">
+      <c r="G11" s="27">
+        <v>20</v>
+      </c>
+      <c r="H11" s="27">
+        <v>24</v>
+      </c>
+      <c r="I11" s="27">
+        <v>46</v>
+      </c>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="23" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="K11" s="23" t="str">
+      <c r="M11" s="23" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L11" s="22">
+      <c r="N11" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$135,Test_Logs!$B$9:$B$135,$B11)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="22">
+      <c r="O11" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$135,Test_Logs!$B$9:$B$135,$B11)</f>
         <v>0</v>
       </c>
-      <c r="N11" s="22">
+      <c r="P11" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$135,Test_Logs!$B$9:$B$135,$B11)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="22">
+      <c r="Q11" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B11)</f>
         <v>0</v>
       </c>
-      <c r="P11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="R11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="15">
         <v>5</v>
       </c>
@@ -1114,32 +1170,37 @@
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="23" t="str">
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="23" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="K12" s="23" t="str">
+      <c r="M12" s="23" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L12" s="22">
+      <c r="N12" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$135,Test_Logs!$B$9:$B$135,$B12)</f>
         <v>0</v>
       </c>
-      <c r="M12" s="22">
+      <c r="O12" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$135,Test_Logs!$B$9:$B$135,$B12)</f>
         <v>0</v>
       </c>
-      <c r="N12" s="22">
+      <c r="P12" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$135,Test_Logs!$B$9:$B$135,$B12)</f>
         <v>0</v>
       </c>
-      <c r="O12" s="22">
+      <c r="Q12" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B12)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="R12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" s="15">
         <v>6</v>
       </c>
@@ -1150,32 +1211,34 @@
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="23" t="str">
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="23" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="K13" s="23" t="str">
+      <c r="M13" s="23" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L13" s="22">
+      <c r="N13" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$135,Test_Logs!$B$9:$B$135,$B13)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="22">
+      <c r="O13" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$135,Test_Logs!$B$9:$B$135,$B13)</f>
         <v>0</v>
       </c>
-      <c r="N13" s="22">
+      <c r="P13" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$135,Test_Logs!$B$9:$B$135,$B13)</f>
         <v>0</v>
       </c>
-      <c r="O13" s="22">
+      <c r="Q13" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B14" s="15">
         <v>7</v>
       </c>
@@ -1186,32 +1249,34 @@
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
-      <c r="J14" s="23" t="str">
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="23" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="K14" s="23" t="str">
+      <c r="M14" s="23" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L14" s="22">
+      <c r="N14" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$135,Test_Logs!$B$9:$B$135,$B14)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="22">
+      <c r="O14" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$135,Test_Logs!$B$9:$B$135,$B14)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="22">
+      <c r="P14" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$135,Test_Logs!$B$9:$B$135,$B14)</f>
         <v>0</v>
       </c>
-      <c r="O14" s="22">
+      <c r="Q14" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B15" s="15">
         <v>8</v>
       </c>
@@ -1222,27 +1287,29 @@
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
-      <c r="J15" s="23" t="str">
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="23" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="K15" s="23" t="str">
+      <c r="M15" s="23" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L15" s="22">
+      <c r="N15" s="22">
         <f>SUMIFS(Test_Logs!F$9:F$135,Test_Logs!$B$9:$B$135,$B15)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="22">
+      <c r="O15" s="22">
         <f>SUMIFS(Test_Logs!G$9:G$135,Test_Logs!$B$9:$B$135,$B15)</f>
         <v>0</v>
       </c>
-      <c r="N15" s="22">
+      <c r="P15" s="22">
         <f>SUMIFS(Test_Logs!H$9:H$135,Test_Logs!$B$9:$B$135,$B15)</f>
         <v>0</v>
       </c>
-      <c r="O15" s="22">
+      <c r="Q15" s="22">
         <f>SUMIFS(Test_Logs!I$9:I$135,Test_Logs!$B$9:$B$135,$B15)</f>
         <v>0</v>
       </c>
@@ -1257,9 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67C8FC6-D7B6-46A9-9A06-D0E7B7D96350}">
   <dimension ref="B1:Y169"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>